<commit_message>
arauco y anastacia auspiciadores
</commit_message>
<xml_diff>
--- a/programa evic2021.xlsx
+++ b/programa evic2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\evic2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B56387A-76DA-44F7-BD90-11BC3F3859E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAAAFAF-6D27-4E1E-88B9-F06BD8FB7494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>KS1</t>
   </si>
@@ -249,6 +249,26 @@
   </si>
   <si>
     <t>HORARIO</t>
+  </si>
+  <si>
+    <t>SPONSOR PRESENTATION 
+ANASTASIA 
+Pablo Zegers</t>
+  </si>
+  <si>
+    <t>SPONSOR PRESENTATION 
+ARAUCO 
+Pablo Vera Cadenas</t>
+  </si>
+  <si>
+    <t>PRESENTACIÓN AUSPICIADOR
+ ANASTASIA 
+Pablo Zegers</t>
+  </si>
+  <si>
+    <t>PRESENTACIÓN AUSPICIADOR
+ARAUCO 
+Pablo Vera Cadenas</t>
   </si>
 </sst>
 </file>
@@ -356,7 +376,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -536,11 +556,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -611,9 +651,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -623,50 +660,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D5:U29"/>
+  <dimension ref="D5:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,7 +1026,8 @@
     <col min="4" max="4" width="11.44140625" style="3"/>
     <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="10" width="34.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="34.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.109375" customWidth="1"/>
     <col min="11" max="12" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="43.77734375" customWidth="1"/>
     <col min="14" max="14" width="20.77734375" customWidth="1"/>
@@ -967,10 +1035,11 @@
     <col min="16" max="16" width="34.109375" hidden="1" customWidth="1"/>
     <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="3.109375" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -981,12 +1050,12 @@
       <c r="K5" s="6"/>
       <c r="L5" s="27"/>
     </row>
-    <row r="6" spans="4:21" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:22" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="5"/>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="12" t="s">
         <v>11</v>
       </c>
@@ -997,17 +1066,17 @@
         <v>13</v>
       </c>
       <c r="J6" s="12"/>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="L6" s="29" t="s">
         <v>45</v>
       </c>
       <c r="M6" s="27"/>
-      <c r="N6" s="48" t="s">
+      <c r="N6" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="O6" s="35"/>
+      <c r="O6" s="42"/>
       <c r="P6" s="12" t="s">
         <v>11</v>
       </c>
@@ -1018,19 +1087,19 @@
         <v>13</v>
       </c>
       <c r="S6" s="12"/>
-      <c r="T6" s="29" t="s">
+      <c r="T6" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="U6" s="30" t="s">
+      <c r="U6" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="4:21" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:22" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="7"/>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="14" t="s">
         <v>0</v>
       </c>
@@ -1041,15 +1110,17 @@
         <v>2</v>
       </c>
       <c r="J7" s="14"/>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="L7" s="28"/>
+      <c r="L7" s="55" t="s">
+        <v>67</v>
+      </c>
       <c r="M7" s="27"/>
-      <c r="N7" s="42" t="s">
+      <c r="N7" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="43"/>
+      <c r="O7" s="38"/>
       <c r="P7" s="14" t="s">
         <v>0</v>
       </c>
@@ -1060,481 +1131,513 @@
         <v>2</v>
       </c>
       <c r="S7" s="14"/>
-      <c r="T7" s="21" t="s">
+      <c r="T7" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="U7" s="28"/>
-    </row>
-    <row r="8" spans="4:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="U7" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="V7" s="27"/>
+    </row>
+    <row r="8" spans="4:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="7"/>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="27"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="36"/>
+      <c r="U8" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="4:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="7"/>
+      <c r="E9" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="12" t="s">
+      <c r="F9" s="51"/>
+      <c r="G9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="15" t="s">
+      <c r="J9" s="12"/>
+      <c r="K9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="L9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="44" t="s">
+      <c r="N9" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="44"/>
-      <c r="P8" s="12" t="s">
+      <c r="O9" s="51"/>
+      <c r="P9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="Q9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="R9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="S8" s="12"/>
-      <c r="T8" s="15" t="s">
+      <c r="S9" s="12"/>
+      <c r="T9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="U8" s="16" t="s">
+      <c r="U9" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="4:21" ht="30" x14ac:dyDescent="0.3">
-      <c r="D9" s="7"/>
-      <c r="E9" s="42" t="s">
+    <row r="10" spans="4:22" ht="30" x14ac:dyDescent="0.3">
+      <c r="D10" s="7"/>
+      <c r="E10" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="14" t="s">
+      <c r="F10" s="50"/>
+      <c r="G10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="21" t="s">
+      <c r="J10" s="14"/>
+      <c r="K10" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="L9" s="47" t="s">
+      <c r="L10" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="N10" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="43"/>
-      <c r="P9" s="14" t="s">
+      <c r="O10" s="50"/>
+      <c r="P10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="R10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="S9" s="14"/>
-      <c r="T9" s="21" t="s">
+      <c r="S10" s="14"/>
+      <c r="T10" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="U9" s="47" t="s">
+      <c r="U10" s="34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="4:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D10" s="7"/>
-      <c r="E10" s="46" t="s">
+    <row r="11" spans="4:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="7"/>
+      <c r="E11" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="45"/>
-      <c r="G10" s="17" t="s">
+      <c r="F11" s="52"/>
+      <c r="G11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="36" t="s">
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="37"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="46" t="s">
+      <c r="L11" s="44"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="45"/>
-      <c r="P10" s="17" t="s">
+      <c r="O11" s="52"/>
+      <c r="P11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="36" t="s">
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="U10" s="37"/>
-    </row>
-    <row r="11" spans="4:21" ht="30" x14ac:dyDescent="0.3">
-      <c r="D11" s="7"/>
-      <c r="E11" s="42" t="s">
+      <c r="U11" s="44"/>
+    </row>
+    <row r="12" spans="4:22" ht="30" x14ac:dyDescent="0.3">
+      <c r="D12" s="7"/>
+      <c r="E12" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="38" t="s">
+      <c r="F12" s="50"/>
+      <c r="G12" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="21" t="s">
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="47" t="s">
+      <c r="L12" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="N11" s="42" t="s">
+      <c r="N12" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="O11" s="43"/>
-      <c r="P11" s="38" t="s">
+      <c r="O12" s="50"/>
+      <c r="P12" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="21" t="s">
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="U11" s="47" t="s">
+      <c r="U12" s="34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="4:21" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="25"/>
-      <c r="E12" s="44" t="s">
+    <row r="13" spans="4:22" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="25"/>
+      <c r="E13" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="44"/>
-      <c r="G12" s="19" t="s">
+      <c r="F13" s="51"/>
+      <c r="G13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K13" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="L12" s="37"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="45" t="s">
+      <c r="L13" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="32"/>
+      <c r="N13" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="44"/>
-      <c r="P12" s="19" t="s">
+      <c r="O13" s="51"/>
+      <c r="P13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="Q12" s="20" t="s">
+      <c r="Q13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R12" s="20" t="s">
+      <c r="R13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="S12" s="20" t="s">
+      <c r="S13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="T12" s="36" t="s">
+      <c r="T13" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="U12" s="37"/>
-    </row>
-    <row r="13" spans="4:21" ht="30" x14ac:dyDescent="0.3">
-      <c r="D13" s="7"/>
-      <c r="E13" s="42" t="s">
+      <c r="U13" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="V13" s="27"/>
+    </row>
+    <row r="14" spans="4:22" ht="30" x14ac:dyDescent="0.3">
+      <c r="D14" s="7"/>
+      <c r="E14" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="21" t="s">
+      <c r="F14" s="50"/>
+      <c r="G14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="39" t="s">
+      <c r="I14" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="21" t="s">
+      <c r="J14" s="13"/>
+      <c r="K14" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="47" t="s">
+      <c r="L14" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="42" t="s">
+      <c r="N14" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="O13" s="43"/>
-      <c r="P13" s="21" t="s">
+      <c r="O14" s="50"/>
+      <c r="P14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="Q13" s="21" t="s">
+      <c r="Q14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="R13" s="39" t="s">
+      <c r="R14" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="S13" s="13"/>
-      <c r="T13" s="21" t="s">
+      <c r="S14" s="13"/>
+      <c r="T14" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="U13" s="47" t="s">
+      <c r="U14" s="34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="4:21" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="7"/>
-      <c r="E14" s="44" t="s">
+    <row r="15" spans="4:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="7"/>
+      <c r="E15" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="20" t="s">
+      <c r="F15" s="51"/>
+      <c r="G15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="39"/>
-      <c r="J14" s="13" t="s">
+      <c r="I15" s="46"/>
+      <c r="J15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="40" t="s">
+      <c r="K15" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="41"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="45" t="s">
+      <c r="L15" s="48"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="O14" s="44"/>
-      <c r="P14" s="20" t="s">
+      <c r="O15" s="51"/>
+      <c r="P15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="Q14" s="20" t="s">
+      <c r="Q15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R14" s="39"/>
-      <c r="S14" s="13" t="s">
+      <c r="R15" s="46"/>
+      <c r="S15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="T14" s="40" t="s">
+      <c r="T15" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="U14" s="41"/>
-    </row>
-    <row r="15" spans="4:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="4"/>
-      <c r="E15" s="42" t="s">
+      <c r="U15" s="48"/>
+    </row>
+    <row r="16" spans="4:22" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="4"/>
+      <c r="E16" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="22" t="s">
+      <c r="F16" s="50"/>
+      <c r="G16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="21" t="s">
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="47" t="s">
+      <c r="L16" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="N15" s="42" t="s">
+      <c r="N16" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="O15" s="43"/>
-      <c r="P15" s="22" t="s">
+      <c r="O16" s="50"/>
+      <c r="P16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="Q15" s="22" t="s">
+      <c r="Q16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="21" t="s">
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="U15" s="47" t="s">
+      <c r="U16" s="34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="4:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E16" s="44" t="s">
+    <row r="17" spans="5:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E17" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="44"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="24" t="s">
+      <c r="F17" s="51"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="N16" s="44" t="s">
+      <c r="N17" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="O16" s="44"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="24" t="s">
+      <c r="O17" s="51"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="K17" s="27"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="11">
+    <row r="18" spans="5:21" x14ac:dyDescent="0.3">
+      <c r="K18" s="27"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="11">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="18" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="N18" s="11"/>
-      <c r="O18" s="11">
-        <v>0.42708333333333337</v>
-      </c>
-    </row>
-    <row r="19" spans="7:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:21" x14ac:dyDescent="0.3">
       <c r="N19" s="11"/>
       <c r="O19" s="11">
-        <v>0.46875000000000006</v>
-      </c>
-    </row>
-    <row r="20" spans="7:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>20</v>
-      </c>
+        <v>0.42708333333333337</v>
+      </c>
+    </row>
+    <row r="20" spans="5:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N20" s="11"/>
       <c r="O20" s="11">
-        <v>0.47916666666666674</v>
-      </c>
-    </row>
-    <row r="21" spans="7:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G21" s="8" t="s">
-        <v>10</v>
+        <v>0.46875000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="5:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="N21" s="11"/>
       <c r="O21" s="11">
-        <v>0.54166666666666674</v>
-      </c>
-    </row>
-    <row r="22" spans="7:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.47916666666666674</v>
+      </c>
+    </row>
+    <row r="22" spans="5:21" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N22" s="11"/>
       <c r="O22" s="11">
-        <v>0.60416666666666674</v>
-      </c>
-    </row>
-    <row r="23" spans="7:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.54166666666666674</v>
+      </c>
+    </row>
+    <row r="23" spans="5:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
       <c r="N23" s="11"/>
       <c r="O23" s="11">
-        <v>0.67361111111111116</v>
-      </c>
-    </row>
-    <row r="24" spans="7:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H24" t="s">
-        <v>17</v>
-      </c>
+        <v>0.60416666666666674</v>
+      </c>
+    </row>
+    <row r="24" spans="5:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N24" s="11"/>
       <c r="O24" s="11">
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="25" spans="7:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.67361111111111116</v>
+      </c>
+    </row>
+    <row r="25" spans="5:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N25" s="11"/>
       <c r="O25" s="11">
-        <v>0.75694444444444442</v>
-      </c>
-    </row>
-    <row r="26" spans="7:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H26" s="10" t="s">
-        <v>19</v>
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="26" spans="5:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>18</v>
       </c>
       <c r="N26" s="11"/>
       <c r="O26" s="11">
+        <v>0.75694444444444442</v>
+      </c>
+    </row>
+    <row r="27" spans="5:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11">
         <v>0.81944444444444442</v>
       </c>
     </row>
-    <row r="27" spans="7:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H27" s="9" t="s">
+    <row r="28" spans="5:21" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="7:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="7:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G29" s="2" t="s">
+    <row r="29" spans="5:21" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="5:21" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H30" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="N17:O17"/>
     <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N14:O14"/>
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="T7:T8"/>
     <mergeCell ref="N6:O6"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="T14:U14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>